<commit_message>
Update to higher CCS transportation and storage costs
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCSTaSC/CCS Transportation and Storage Cost.xlsx
+++ b/InputData/ccs/CCSTaSC/CCS Transportation and Storage Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CCSTaSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\CCSTaSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB69C57-C5D6-459F-AF6B-9308998FBC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7C928A-3AAF-49BE-9925-7B059DEE51E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21525" yWindow="2850" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <t>Value from study (2021 $)</t>
   </si>
   <si>
-    <t>2021 to 2012 $</t>
+    <t>2018 to 2012 $</t>
   </si>
 </sst>
 </file>
@@ -123,7 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -137,7 +137,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,7 +445,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
@@ -501,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,12 +508,15 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.84699999999999998</v>
+        <v>0.9143273584567535</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{E6E6B16C-F4E4-4E8F-9F7E-3FD9DA689F40}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -525,8 +527,8 @@
   </sheetPr>
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,125 +633,125 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="C2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="D2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="E2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="F2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="G2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="H2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="I2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="J2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="K2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="L2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="M2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="N2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="O2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="P2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="Q2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="R2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="S2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="T2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="U2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="V2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="W2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="X2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="Y2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="Z2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="AA2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="AB2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="AC2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="AD2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
-      </c>
-      <c r="AE2" s="7">
-        <f>About!$B$10*About!$B$11</f>
-        <v>14.398999999999999</v>
+      <c r="B2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="C2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="D2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="E2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="F2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="G2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="H2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="I2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="J2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="K2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="L2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="M2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="N2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="O2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="P2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="Q2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="R2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="S2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="T2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="U2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="V2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="W2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="X2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="Y2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="Z2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="AA2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="AB2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="AC2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="AD2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
+      </c>
+      <c r="AE2">
+        <f>About!$B$10*About!$B$11</f>
+        <v>21.02952924450533</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>